<commit_message>
KIBON-250: InstitutionStammdaten: Felder oeffnungstage und oeffnungsstunden entfernen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8401F49-334C-4E65-9492-4EE9E14F0DEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11805" windowHeight="5850"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11805" windowHeight="5850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -17,12 +23,19 @@
     <definedName name="verguenstigung">Data!$P$9</definedName>
     <definedName name="vollkosten">Data!$N$9</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Parameter</t>
   </si>
@@ -90,9 +103,6 @@
     <t>Kosten in CHF</t>
   </si>
   <si>
-    <t>Öffnungstage</t>
-  </si>
-  <si>
     <t>{auswertungVon}</t>
   </si>
   <si>
@@ -127,9 +137,6 @@
   </si>
   <si>
     <t>{institution}</t>
-  </si>
-  <si>
-    <t>{oeffnungstage}</t>
   </si>
   <si>
     <t>{repeatKantonRow}</t>
@@ -138,11 +145,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,38 +340,38 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Dezimal" xfId="1" builtinId="3"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,9 +388,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -421,9 +428,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,9 +462,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,9 +514,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,17 +707,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
@@ -691,25 +734,24 @@
     <col min="14" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -718,7 +760,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,23 +769,23 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
@@ -753,65 +795,62 @@
       <c r="C7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="23" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="27"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="23" t="s">
+      <c r="O7" s="25"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="S7" s="23" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="29"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="27"/>
       <c r="N8" s="17" t="s">
         <v>9</v>
       </c>
@@ -821,31 +860,30 @@
       <c r="P8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="H9" s="12" t="e">
         <f>E9-DAY(E9)+1</f>
@@ -876,26 +914,23 @@
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="Q9" s="3" t="e">
         <f>IF(E9&gt;EOMONTH(D9,12),"Nein","Ja")</f>
         <v>#VALUE!</v>
       </c>
       <c r="R9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="T9" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
@@ -931,18 +966,21 @@
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="S7:S8"/>
+  <mergeCells count="16">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="E7:E8"/>
@@ -954,11 +992,6 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-120: Kanton statistic translated
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8401F49-334C-4E65-9492-4EE9E14F0DEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF7CE0-B361-4DCE-8D3E-32D7E98FE246}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="11805" windowHeight="5850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,11 +23,12 @@
     <definedName name="verguenstigung">Data!$P$9</definedName>
     <definedName name="vollkosten">Data!$N$9</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,61 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Von</t>
-  </si>
-  <si>
-    <t>Bis</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>BG-ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>BG-Pensum</t>
-  </si>
-  <si>
-    <t>Vollkosten</t>
-  </si>
-  <si>
-    <t>Elternbeitrag</t>
-  </si>
-  <si>
-    <t>Gutschein</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Kantonsabrechnung Plätze und Elternbeiträge</t>
-  </si>
-  <si>
-    <t>Bebéfaktor</t>
-  </si>
-  <si>
-    <t>Platzbelegung aufgrund der Tage</t>
-  </si>
-  <si>
-    <t>Monatsanfang</t>
-  </si>
-  <si>
-    <t>Monatsende</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Nettoarbeitstage Monat</t>
   </si>
@@ -100,9 +47,6 @@
     <t>Anteil des Monats</t>
   </si>
   <si>
-    <t>Kosten in CHF</t>
-  </si>
-  <si>
     <t>{auswertungVon}</t>
   </si>
   <si>
@@ -140,6 +84,69 @@
   </si>
   <si>
     <t>{repeatKantonRow}</t>
+  </si>
+  <si>
+    <t>{parameterTitle}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
+    <t>{fallIdTitle}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{geburtsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{betreuungVonTitle}</t>
+  </si>
+  <si>
+    <t>{betreuungBisTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensumTitle}</t>
+  </si>
+  <si>
+    <t>{babyFaktorTitle}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{kantonTitle}</t>
+  </si>
+  <si>
+    <t>{monatsanfangTitle}</t>
+  </si>
+  <si>
+    <t>{monatsendeTitle}</t>
+  </si>
+  <si>
+    <t>{platzbelegungTageTitle}</t>
+  </si>
+  <si>
+    <t>{kostenCHFTitle}</t>
+  </si>
+  <si>
+    <t>{vollkostenTitle}</t>
+  </si>
+  <si>
+    <t>{elternbeitragTitle}</t>
+  </si>
+  <si>
+    <t>{gutscheinTitle}</t>
+  </si>
+  <si>
+    <t>{totalTitle}</t>
   </si>
 </sst>
 </file>
@@ -149,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +186,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -292,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +354,9 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -346,9 +364,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -369,6 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -714,7 +730,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +769,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="7"/>
@@ -761,8 +777,8 @@
       <c r="E1" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+      <c r="A3" s="30" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="8"/>
@@ -771,80 +787,80 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>6</v>
+      <c r="A7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E7" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="L7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>20</v>
-      </c>
       <c r="M7" s="27" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="O7" s="25"/>
       <c r="P7" s="26"/>
-      <c r="Q7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7" s="20" t="s">
-        <v>12</v>
+      <c r="Q7" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="22"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="29"/>
@@ -852,38 +868,38 @@
       <c r="L8" s="29"/>
       <c r="M8" s="27"/>
       <c r="N8" s="17" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
+        <v>35</v>
+      </c>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H9" s="12" t="e">
         <f>E9-DAY(E9)+1</f>
@@ -914,25 +930,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="Q9" s="3" t="e">
-        <f>IF(E9&gt;EOMONTH(D9,12),"Nein","Ja")</f>
+        <f>IF(E9&gt;EOMONTH(D9,12),"","X")</f>
         <v>#VALUE!</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="S9" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>

</xml_diff>

<commit_message>
KIBON-1171: Statistik Kanton angepasst mit Kantons- und Gemeindegutschein
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\TODO\KIBON-REPORTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F8B36B-A57A-48C8-9654-2AF2DBD1A1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4886E6CB-E935-4D83-8124-66E88687A72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <definedName name="bgPensum">Data!$H$9</definedName>
     <definedName name="elternbeitrag">Data!$P$9</definedName>
     <definedName name="platzbelegungAufgrundTage">Data!$N$9</definedName>
-    <definedName name="verguenstigung">Data!$Q$9</definedName>
+    <definedName name="verguenstigung">Data!$S$9</definedName>
+    <definedName name="verguenstigungGemeinde">Data!$R$9</definedName>
+    <definedName name="verguenstigungKanton">Data!$Q$9</definedName>
     <definedName name="vollkosten">Data!$O$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Anteil des Monats</t>
   </si>
@@ -73,9 +75,6 @@
     <t>{elternbeitrag}</t>
   </si>
   <si>
-    <t>{verguenstigung}</t>
-  </si>
-  <si>
     <t>{institution}</t>
   </si>
   <si>
@@ -139,9 +138,6 @@
     <t>{elternbeitragTitle}</t>
   </si>
   <si>
-    <t>{gutscheinTitle}</t>
-  </si>
-  <si>
     <t>{totalTitle}</t>
   </si>
   <si>
@@ -155,6 +151,24 @@
   </si>
   <si>
     <t>Tage Intervall</t>
+  </si>
+  <si>
+    <t>{gutscheinKantonTitel}</t>
+  </si>
+  <si>
+    <t>{gutscheinGemeindeTitel}</t>
+  </si>
+  <si>
+    <t>{gutscheinTotalTitel}</t>
+  </si>
+  <si>
+    <t>{verguenstigungKanton}</t>
+  </si>
+  <si>
+    <t>{verguenstigungGemeinde}</t>
+  </si>
+  <si>
+    <t>{verguenstigungTotal}</t>
   </si>
 </sst>
 </file>
@@ -367,34 +381,34 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -738,47 +752,47 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="6" customWidth="1"/>
-    <col min="15" max="17" width="12.6640625" customWidth="1"/>
-    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="21" max="21" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -786,9 +800,9 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="1"/>
@@ -796,107 +810,115 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="24" t="s">
+      <c r="L7" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="25" t="s">
+      <c r="U7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S7" s="25" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="31"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="17" t="s">
-        <v>32</v>
-      </c>
       <c r="Q8" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>3</v>
@@ -944,29 +966,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="15" t="e">
-        <f>P9+Q9</f>
+        <f>P9+S9</f>
         <v>#VALUE!</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9" s="3" t="e">
+        <v>40</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="3" t="e">
         <f>IF(F9&gt;EOMONTH(E9,12),"","X")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="U9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" t="s">
         <v>12</v>
       </c>
-      <c r="T9" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="9"/>
@@ -996,39 +1024,47 @@
         <v>0</v>
       </c>
       <c r="Q10" s="19">
+        <f>SUM(verguenstigungKanton)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="19">
+        <f>SUM(verguenstigungGemeinde)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="19">
         <f>SUM(verguenstigung)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O7:S7"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="R7:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2009: Excel Report angepasst, Total Zeile Weg
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\KibonReports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3559E0C-BEA4-4F5C-B25A-826C34922490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C3794-520F-49D9-9E61-CEB5C526814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Anteil des Monats</t>
   </si>
@@ -77,9 +77,6 @@
     <t>{institution}</t>
   </si>
   <si>
-    <t>{repeatKantonRow}</t>
-  </si>
-  <si>
     <t>{parameterTitle}</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>{elternbeitragTitle}</t>
   </si>
   <si>
-    <t>{totalTitle}</t>
-  </si>
-  <si>
     <t>{gemeindeTitle}</t>
   </si>
   <si>
@@ -183,6 +177,9 @@
   </si>
   <si>
     <t>{bgPensumTotal}</t>
+  </si>
+  <si>
+    <t>{repeatRow}</t>
   </si>
 </sst>
 </file>
@@ -343,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,12 +356,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -384,25 +375,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -423,9 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -769,48 +751,50 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16" style="6" customWidth="1"/>
-    <col min="17" max="21" width="12.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.28515625" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="6" customWidth="1"/>
+    <col min="17" max="21" width="12.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.33203125" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -818,200 +802,200 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="21"/>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="25" t="s">
+      <c r="N7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="30" t="s">
+      <c r="W7" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="30" t="s">
+      <c r="T8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="W7" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="U8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
     </row>
-    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="T8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="12" t="e">
+      <c r="K9" s="10" t="e">
         <f>F9-DAY(F9)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L9" s="12" t="e">
+      <c r="L9" s="10" t="e">
         <f>EOMONTH(F9,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M9" s="14" t="e">
+      <c r="M9" s="12" t="e">
         <f>L9-K9+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N9" s="14" t="e">
+      <c r="N9" s="12" t="e">
         <f>G9-F9+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O9" s="14" t="e">
+      <c r="O9" s="12" t="e">
         <f>N9/M9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P9" s="13" t="e">
+      <c r="P9" s="11" t="e">
         <f>J9*O9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="15" t="e">
+      <c r="Q9" s="13" t="e">
         <f>R9+U9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R9" s="16" t="s">
+      <c r="R9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="V9" s="3" t="e">
         <f>IF(F9&gt;EOMONTH(E9,12),"","X")</f>
@@ -1021,76 +1005,11 @@
         <v>10</v>
       </c>
       <c r="X9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="18">
-        <f>SUM(bgPensumKanton)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
-        <f>SUM(bgPensumGemeinde)</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="18">
-        <f>SUM(bgPensum)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="18" t="e">
-        <f>SUM(platzbelegungAufgrundTage)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q10" s="19" t="e">
-        <f>SUM(vollkosten)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R10" s="19">
-        <f>SUM(elternbeitrag)</f>
-        <v>0</v>
-      </c>
-      <c r="S10" s="19">
-        <f>SUM(verguenstigungKanton)</f>
-        <v>0</v>
-      </c>
-      <c r="T10" s="19">
-        <f>SUM(verguenstigungGemeinde)</f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="19">
-        <f>SUM(verguenstigung)</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A7:A8"/>
@@ -1107,6 +1026,9 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2031: Kanton Statistik wurde ergaenzt mit zwei neuen Kolumne, einen Total und einen neuen Parameter fuer die Selbstbehalt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C3794-520F-49D9-9E61-CEB5C526814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0DC1AF-064C-4376-86C6-722BC77544F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="anteilMonat">Data!$O$9</definedName>
-    <definedName name="bgPensum">Data!$J$9</definedName>
-    <definedName name="bgPensumGemeinde">Data!$I$9</definedName>
-    <definedName name="bgPensumKanton">Data!$H$9</definedName>
-    <definedName name="elternbeitrag">Data!$R$9</definedName>
-    <definedName name="platzbelegungAufgrundTage">Data!$P$9</definedName>
-    <definedName name="verguenstigung">Data!$U$9</definedName>
-    <definedName name="verguenstigungGemeinde">Data!$T$9</definedName>
-    <definedName name="verguenstigungKanton">Data!$S$9</definedName>
-    <definedName name="vollkosten">Data!$Q$9</definedName>
+    <definedName name="anteilMonat">Data!$Q$10</definedName>
+    <definedName name="bgPensum">Data!$J$10</definedName>
+    <definedName name="bgPensumGemeinde">Data!$I$10</definedName>
+    <definedName name="bgPensumKanton">Data!$H$10</definedName>
+    <definedName name="elternbeitrag">Data!$T$10</definedName>
+    <definedName name="platzbelegungAufgrundTage">Data!$R$10</definedName>
+    <definedName name="verguenstigung">Data!$W$10</definedName>
+    <definedName name="verguenstigungGemeinde">Data!$V$10</definedName>
+    <definedName name="verguenstigungKanton">Data!$U$10</definedName>
+    <definedName name="vollkosten">Data!$S$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Anteil des Monats</t>
   </si>
@@ -180,14 +180,28 @@
   </si>
   <si>
     <t>{repeatRow}</t>
+  </si>
+  <si>
+    <t>{kantonSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{kantonSelbstbehaltTitle}</t>
+  </si>
+  <si>
+    <t>{anteilKalenderjahrTitle}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -340,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -379,6 +393,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -386,9 +416,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,12 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,48 +772,51 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="6" customWidth="1"/>
-    <col min="17" max="21" width="12.6640625" customWidth="1"/>
-    <col min="22" max="22" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.33203125" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" style="6" customWidth="1"/>
+    <col min="19" max="23" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" customWidth="1"/>
+    <col min="27" max="27" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -802,7 +826,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
@@ -812,7 +836,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -820,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -828,207 +852,233 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G8" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I8" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="N8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="O8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="P8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="Q8" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="25" t="s">
+      <c r="R8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="S8" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="18" t="s">
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="18" t="s">
+      <c r="Y8" s="24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="15" t="s">
+    <row r="9" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="T9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="15" t="s">
+      <c r="U9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="V9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="15" t="s">
+      <c r="W9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="10" t="e">
-        <f>F9-DAY(F9)+1</f>
+      <c r="K10" s="19" t="e">
+        <f>J10/12*Q10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L9" s="10" t="e">
-        <f>EOMONTH(F9,0)</f>
+      <c r="L10" s="18" t="e">
+        <f>K10*$B$6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M9" s="12" t="e">
-        <f>L9-K9+1</f>
+      <c r="M10" s="10" t="e">
+        <f>F10-DAY(F10)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N9" s="12" t="e">
-        <f>G9-F9+1</f>
+      <c r="N10" s="10" t="e">
+        <f>EOMONTH(F10,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O9" s="12" t="e">
-        <f>N9/M9</f>
+      <c r="O10" s="12" t="e">
+        <f>N10-M10+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P9" s="11" t="e">
-        <f>J9*O9</f>
+      <c r="P10" s="12" t="e">
+        <f>G10-F10+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q9" s="13" t="e">
-        <f>R9+U9</f>
+      <c r="Q10" s="12" t="e">
+        <f>P10/O10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R10" s="11" t="e">
+        <f>J10*Q10</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S10" s="13" t="e">
+        <f>T10+W10</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="U10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="T9" s="14" t="s">
+      <c r="V10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="U9" s="14" t="s">
+      <c r="W10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="V9" s="3" t="e">
-        <f>IF(F9&gt;EOMONTH(E9,12),"","X")</f>
+      <c r="X10" s="3" t="e">
+        <f>IF(F10&gt;EOMONTH(E10,12),"","X")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="Y10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z10" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
+  <mergeCells count="21">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="S8:W8"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2068 fix some formulas
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0DC1AF-064C-4376-86C6-722BC77544F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A1A49D-1102-40E9-AAC4-838E3E2F6546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -354,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,9 +391,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -774,49 +771,47 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" style="6" customWidth="1"/>
-    <col min="19" max="23" width="12.6640625" customWidth="1"/>
-    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" style="6" customWidth="1"/>
+    <col min="19" max="23" width="12.7109375" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="21" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -826,7 +821,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
@@ -836,7 +831,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -844,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -852,102 +847,102 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="M8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="S8" s="27" t="s">
+      <c r="S8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="28"/>
-      <c r="U8" s="28"/>
-      <c r="V8" s="28"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="24" t="s">
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="Y8" s="24" t="s">
+      <c r="Y8" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="30"/>
+    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="29"/>
       <c r="S9" s="15" t="s">
         <v>27</v>
       </c>
@@ -963,10 +958,10 @@
       <c r="W9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -997,11 +992,11 @@
       <c r="J10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="19" t="e">
-        <f>J10/12*Q10</f>
+      <c r="K10" s="18" t="e">
+        <f>H10/12*Q10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L10" s="18" t="e">
+      <c r="L10" s="12" t="e">
         <f>K10*$B$6</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
KIBON-2068: FR Uebersetzungen + neue Titlen fuer die die waren noch hardcodiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A1A49D-1102-40E9-AAC4-838E3E2F6546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B954A-19F8-4983-AB9E-75F776C986BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -44,9 +44,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
-    <t>Anteil des Monats</t>
-  </si>
-  <si>
     <t>{auswertungVon}</t>
   </si>
   <si>
@@ -137,12 +134,6 @@
     <t>{gemeinde}</t>
   </si>
   <si>
-    <t>Tage Monat</t>
-  </si>
-  <si>
-    <t>Tage Intervall</t>
-  </si>
-  <si>
     <t>{gutscheinKantonTitel}</t>
   </si>
   <si>
@@ -192,6 +183,15 @@
   </si>
   <si>
     <t>{selbstbehaltTitle}</t>
+  </si>
+  <si>
+    <t>{tageMonatTitle}</t>
+  </si>
+  <si>
+    <t>{tageIntervallTitle}</t>
+  </si>
+  <si>
+    <t>{anteilMonatKantonTitle}</t>
   </si>
 </sst>
 </file>
@@ -771,49 +771,51 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" style="6" customWidth="1"/>
-    <col min="19" max="23" width="12.7109375" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.28515625" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" style="6" customWidth="1"/>
+    <col min="19" max="23" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" customWidth="1"/>
+    <col min="27" max="27" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="21" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -821,9 +823,9 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="1"/>
@@ -831,100 +833,100 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="20" t="s">
+      <c r="P8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="Q8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="25" t="s">
+      <c r="R8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="29" t="s">
+      <c r="S8" s="26" t="s">
         <v>25</v>
-      </c>
-      <c r="S8" s="26" t="s">
-        <v>26</v>
       </c>
       <c r="T8" s="27"/>
       <c r="U8" s="27"/>
       <c r="V8" s="27"/>
       <c r="W8" s="28"/>
       <c r="X8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="Y8" s="23" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -944,53 +946,53 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="29"/>
       <c r="S9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="T9" s="15" t="s">
-        <v>28</v>
-      </c>
       <c r="U9" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="W9" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="X9" s="24"/>
       <c r="Y9" s="24"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>8</v>
-      </c>
       <c r="H10" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K10" s="18" t="e">
         <f>H10/12*Q10</f>
@@ -1029,26 +1031,26 @@
         <v>#VALUE!</v>
       </c>
       <c r="T10" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U10" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="X10" s="3" t="e">
         <f>IF(F10&gt;EOMONTH(E10,12),"","X")</f>
         <v>#VALUE!</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2577: BabyTarif im DB speichern und von DB lesen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B954A-19F8-4983-AB9E-75F776C986BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2848053D-644E-49C4-8B3D-DDA575FB52BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>{auswertungVon}</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>{anteilMonatKantonTitle}</t>
+  </si>
+  <si>
+    <t>{babyTarif}</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -397,35 +400,35 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -771,8 +774,8 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:Q9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,93 +861,93 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="Q8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="29" t="s">
+      <c r="R8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="26" t="s">
+      <c r="S8" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="28"/>
-      <c r="X8" s="23" t="s">
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="23" t="s">
+      <c r="Y8" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="29"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="27"/>
       <c r="S9" s="15" t="s">
         <v>26</v>
       </c>
@@ -960,8 +963,8 @@
       <c r="W9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -1042,9 +1045,8 @@
       <c r="W10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="X10" s="3" t="e">
-        <f>IF(F10&gt;EOMONTH(E10,12),"","X")</f>
-        <v>#VALUE!</v>
+      <c r="X10" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="Y10" s="5" t="s">
         <v>9</v>
@@ -1055,6 +1057,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A8:A9"/>
@@ -1071,11 +1078,6 @@
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>